<commit_message>
changing to use RAST Multiple
</commit_message>
<xml_diff>
--- a/data/RealData/GramDataEdit5.xlsx
+++ b/data/RealData/GramDataEdit5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sagoyal/Documents/kb_genomeclassification/data/RealData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E868300-A084-B34D-BF79-2DEEFCC38AA1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFF98432-C58D-F24A-AAC6-08D37D6B7954}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5960" yWindow="4060" windowWidth="27640" windowHeight="16940" xr2:uid="{E7106E9D-2E29-7B43-B2D2-EBEC496FEBDE}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
   <si>
     <t>N</t>
   </si>
@@ -45,6 +45,24 @@
   </si>
   <si>
     <t>Phenotype</t>
+  </si>
+  <si>
+    <t>References</t>
+  </si>
+  <si>
+    <t>Evidence Types</t>
+  </si>
+  <si>
+    <t>a;b;c</t>
+  </si>
+  <si>
+    <t>d;e;f</t>
+  </si>
+  <si>
+    <t>227asdf882.1</t>
+  </si>
+  <si>
+    <t>10asdf6370.11</t>
   </si>
 </sst>
 </file>
@@ -402,26 +420,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{342FC334-0FD6-FE4E-9B07-483D4E70EC70}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>2</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
         <v>204669.6</v>
       </c>
@@ -429,15 +454,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:4">
       <c r="A3" s="1">
         <v>234267.13</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1">
         <v>240015.3</v>
       </c>
@@ -445,7 +473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:4">
       <c r="A5" s="1">
         <v>1806.1</v>
       </c>
@@ -453,7 +481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:4">
       <c r="A6" s="1">
         <v>83331.100000000006</v>
       </c>
@@ -461,23 +489,26 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="1">
-        <v>106370.11</v>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:4">
       <c r="A8" s="1">
         <v>164756.6</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="1">
         <v>216594.1</v>
       </c>
@@ -485,15 +516,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="1">
-        <v>227882.1</v>
+    <row r="10" spans="1:4">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:4">
       <c r="A11" s="1">
         <v>233413.1</v>
       </c>
@@ -501,7 +532,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:4">
       <c r="A12" s="1">
         <v>246196.1</v>
       </c>
@@ -509,7 +540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:4">
       <c r="A13" s="1">
         <v>262316.09999999998</v>
       </c>

</xml_diff>

<commit_message>
basic build classifier is working
</commit_message>
<xml_diff>
--- a/data/RealData/GramDataEdit5.xlsx
+++ b/data/RealData/GramDataEdit5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sagoyal/Documents/kb_genomeclassification/data/RealData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFF98432-C58D-F24A-AAC6-08D37D6B7954}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0AC7BFC-CE1B-5A45-ACD8-F8D6BBE087A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5960" yWindow="4060" windowWidth="27640" windowHeight="16940" xr2:uid="{E7106E9D-2E29-7B43-B2D2-EBEC496FEBDE}"/>
   </bookViews>
@@ -423,7 +423,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -537,7 +537,7 @@
         <v>246196.1</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:4">

</xml_diff>